<commit_message>
Add the remaining data
</commit_message>
<xml_diff>
--- a/Manual vs LLM.xlsx
+++ b/Manual vs LLM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5fa5fe2a5bf147a6/Desktop/Green LLM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="130" documentId="11_CF8FA6A7534C74F76944A01B7D57F0B67D1070FC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{57751BB0-F5EC-4FC3-A1E0-7B6C55C22F04}"/>
+  <xr:revisionPtr revIDLastSave="176" documentId="11_CF8FA6A7534C74F76944A01B7D57F0B67D1070FC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{141C59E9-9E76-4A6B-97D5-5439F5A9C6EF}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -183,7 +183,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
-    <numFmt numFmtId="172" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -226,7 +226,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -240,9 +240,8 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -259,6 +258,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -440,7 +443,7 @@
   <dimension ref="A1:Q36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,8 +562,8 @@
         <v>3.9606767796499997E-3</v>
       </c>
       <c r="I3" s="5">
-        <f t="shared" si="0"/>
-        <v>1.70855831129E-2</v>
+        <f>SUM(B3:H3)</f>
+        <v>1.7588166848300002E-2</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -1029,7 +1032,7 @@
         <v>27</v>
       </c>
       <c r="B15" s="4">
-        <f t="shared" ref="B15:H15" si="4">SUM(B3,B13,B14)</f>
+        <f t="shared" ref="B15" si="4">SUM(B3,B13,B14)</f>
         <v>5.5433182455644821E-4</v>
       </c>
       <c r="C15" s="4">
@@ -1152,6 +1155,19 @@
       <c r="E19">
         <v>5</v>
       </c>
+      <c r="F19">
+        <v>5</v>
+      </c>
+      <c r="G19">
+        <v>5</v>
+      </c>
+      <c r="H19">
+        <v>5</v>
+      </c>
+      <c r="I19">
+        <f>SUM(B19:H19)</f>
+        <v>31</v>
+      </c>
       <c r="L19" t="s">
         <v>31</v>
       </c>
@@ -1164,13 +1180,26 @@
         <v>1</v>
       </c>
       <c r="C20" s="8">
+        <v>0.04</v>
+      </c>
+      <c r="D20" s="8">
         <v>0</v>
       </c>
-      <c r="D20" s="8">
-        <v>0.1</v>
-      </c>
       <c r="E20" s="8">
-        <v>0.22</v>
+        <v>0</v>
+      </c>
+      <c r="F20" s="8">
+        <v>0</v>
+      </c>
+      <c r="G20" s="8">
+        <v>0</v>
+      </c>
+      <c r="H20" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="I20" s="8">
+        <f>AVERAGE(B20:H20)</f>
+        <v>0.15</v>
       </c>
       <c r="J20" s="2"/>
       <c r="L20">
@@ -1193,6 +1222,19 @@
       <c r="E21">
         <v>3</v>
       </c>
+      <c r="F21">
+        <v>3</v>
+      </c>
+      <c r="G21">
+        <v>3</v>
+      </c>
+      <c r="H21">
+        <v>3</v>
+      </c>
+      <c r="I21">
+        <f>SUM(B21:H21)</f>
+        <v>17</v>
+      </c>
       <c r="L21" t="s">
         <v>34</v>
       </c>
@@ -1208,10 +1250,23 @@
         <v>1</v>
       </c>
       <c r="D22" s="8">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="E22" s="8">
-        <v>0.67</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="F22" s="8">
+        <v>0</v>
+      </c>
+      <c r="G22" s="8">
+        <v>0</v>
+      </c>
+      <c r="H22" s="8">
+        <v>0</v>
+      </c>
+      <c r="I22" s="8">
+        <f>AVERAGE(B22:H22)</f>
+        <v>0.29499999999999998</v>
       </c>
       <c r="L22">
         <v>50</v>
@@ -1237,6 +1292,22 @@
         <f>(E19+E21)*$L$20</f>
         <v>1.7600000000000001E-2</v>
       </c>
+      <c r="F23">
+        <f t="shared" ref="F23:H23" si="12">(F19+F21)*$L$20</f>
+        <v>1.7600000000000001E-2</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="12"/>
+        <v>1.7600000000000001E-2</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="12"/>
+        <v>1.7600000000000001E-2</v>
+      </c>
+      <c r="I23">
+        <f>SUM(B23:H23)</f>
+        <v>0.10560000000000001</v>
+      </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -1246,28 +1317,32 @@
         <v>0</v>
       </c>
       <c r="C24">
-        <f>C2*$L$36</f>
-        <v>842.08</v>
+        <f>C2*$L$36*(1-C20)</f>
+        <v>808.39679999999998</v>
       </c>
       <c r="D24">
-        <f t="shared" ref="C24:H24" si="12">D2*$L$36</f>
+        <f t="shared" ref="D24:H24" si="13">D2*$L$36*(1-D20)</f>
         <v>897.18000000000006</v>
       </c>
       <c r="E24">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>766.84</v>
       </c>
       <c r="F24">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>945.06000000000006</v>
       </c>
       <c r="G24">
-        <f t="shared" si="12"/>
+        <f>G2*$L$36*(1-G20)</f>
         <v>954.94</v>
       </c>
       <c r="H24">
-        <f t="shared" si="12"/>
-        <v>1329.6200000000001</v>
+        <f>H2*$L$36*(1-H20)</f>
+        <v>1316.3238000000001</v>
+      </c>
+      <c r="I24">
+        <f>SUM(B24:H24)</f>
+        <v>5688.7406000000001</v>
       </c>
       <c r="L24" t="s">
         <v>37</v>
@@ -1303,6 +1378,10 @@
         <f>($L$32+$L$34)*(H2*$L$28)</f>
         <v>587.83199999999999</v>
       </c>
+      <c r="I25">
+        <f>SUM(B25:H25)</f>
+        <v>2163.5039999999999</v>
+      </c>
       <c r="L25">
         <v>217</v>
       </c>
@@ -1312,65 +1391,73 @@
         <v>43</v>
       </c>
       <c r="B26">
-        <f>(1-B22)*B2+B25</f>
+        <f t="shared" ref="B26:H26" si="14">(1-B22)*B2+B25</f>
         <v>0</v>
       </c>
       <c r="C26">
-        <f>(1-C22)*C2+C25</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="D26">
-        <f>(1-D22)*D2+D25</f>
-        <v>1104.9480000000001</v>
+        <f t="shared" si="14"/>
+        <v>2757.6480000000001</v>
       </c>
       <c r="E26">
-        <f>(1-E22)*E2+E25</f>
-        <v>1004.9639999999999</v>
+        <f t="shared" si="14"/>
+        <v>2225.8540000000003</v>
       </c>
       <c r="F26">
-        <f>(1-F22)*F2+F25</f>
+        <f t="shared" si="14"/>
         <v>2904.8159999999998</v>
       </c>
       <c r="G26">
-        <f>(1-G22)*G2+G25</f>
+        <f t="shared" si="14"/>
         <v>2935.1840000000002</v>
       </c>
       <c r="H26">
-        <f>(1-H22)*H2+H25</f>
+        <f t="shared" si="14"/>
         <v>4086.8319999999999</v>
+      </c>
+      <c r="I26">
+        <f>SUM(B26:H26)</f>
+        <v>14910.334000000001</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="11">
+      <c r="B27">
         <f>B23+(B24+B26)*$L$2*$N$2</f>
         <v>2.2000000000000001E-3</v>
       </c>
       <c r="C27" s="5">
-        <f t="shared" ref="C27:H27" si="13">C23+(C24+C26)*$L$2*$N$2</f>
-        <v>1.6353188540328002E-2</v>
+        <f t="shared" ref="C27:H27" si="15">C23+(C24+C26)*$L$2*$N$2</f>
+        <v>1.6315060998714881E-2</v>
       </c>
       <c r="D27" s="5">
-        <f t="shared" si="13"/>
-        <v>1.9866299479704801E-2</v>
+        <f t="shared" si="15"/>
+        <v>2.1737065559649802E-2</v>
       </c>
       <c r="E27" s="5">
-        <f t="shared" si="13"/>
-        <v>1.9605585298911401E-2</v>
-      </c>
-      <c r="F27" s="11">
-        <f t="shared" si="13"/>
-        <v>4.3578492362765994E-3</v>
+        <f t="shared" si="15"/>
+        <v>2.0987566057272901E-2</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="15"/>
+        <v>2.19578492362766E-2</v>
       </c>
       <c r="G27" s="4">
-        <f t="shared" si="13"/>
-        <v>4.4034077727234007E-3</v>
-      </c>
-      <c r="H27" s="11">
-        <f t="shared" si="13"/>
-        <v>6.1311276548982E-3</v>
+        <f t="shared" si="15"/>
+        <v>2.2003407772723402E-2</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="15"/>
+        <v>2.3716077083135532E-2</v>
+      </c>
+      <c r="I27">
+        <f>SUM(B27:H27)</f>
+        <v>0.12891702670777314</v>
       </c>
       <c r="L27" t="s">
         <v>38</v>
@@ -1385,28 +1472,32 @@
         <v>0.47740000000000005</v>
       </c>
       <c r="C28">
-        <f t="shared" ref="C28:H28" si="14">C27*$L$25</f>
-        <v>3.5486419132511764</v>
+        <f t="shared" ref="C28:H28" si="16">C27*$L$25</f>
+        <v>3.5403682367211293</v>
       </c>
       <c r="D28">
-        <f t="shared" si="14"/>
-        <v>4.3109869870959416</v>
+        <f t="shared" si="16"/>
+        <v>4.7169432264440072</v>
       </c>
       <c r="E28">
-        <f t="shared" si="14"/>
-        <v>4.2544120098637741</v>
+        <f t="shared" si="16"/>
+        <v>4.5543018344282196</v>
       </c>
       <c r="F28">
-        <f t="shared" si="14"/>
-        <v>0.94565328427202211</v>
+        <f t="shared" si="16"/>
+        <v>4.7648532842720224</v>
       </c>
       <c r="G28">
-        <f t="shared" si="14"/>
-        <v>0.95553948668097799</v>
+        <f t="shared" si="16"/>
+        <v>4.7747394866809785</v>
       </c>
       <c r="H28">
-        <f t="shared" si="14"/>
-        <v>1.3304547011129093</v>
+        <f t="shared" si="16"/>
+        <v>5.1463887270404101</v>
+      </c>
+      <c r="I28">
+        <f>SUM(B28:H28)</f>
+        <v>27.974994795586767</v>
       </c>
       <c r="L28" s="10">
         <v>0.42</v>

</xml_diff>

<commit_message>
Update the excel data sheet
</commit_message>
<xml_diff>
--- a/Manual vs LLM.xlsx
+++ b/Manual vs LLM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5fa5fe2a5bf147a6/Desktop/Green LLM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="176" documentId="11_CF8FA6A7534C74F76944A01B7D57F0B67D1070FC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{141C59E9-9E76-4A6B-97D5-5439F5A9C6EF}"/>
+  <xr:revisionPtr revIDLastSave="282" documentId="11_CF8FA6A7534C74F76944A01B7D57F0B67D1070FC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B0F363E-FCDC-4153-BA03-CE02C71A53E7}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -226,7 +226,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -242,6 +242,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -443,7 +444,7 @@
   <dimension ref="A1:Q36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="I28" sqref="A18:I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,31 +534,31 @@
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="4">
-        <f t="shared" ref="B3:I3" si="0">$L$2*B2*$N$2</f>
+      <c r="B3" s="2">
+        <f t="shared" ref="B3:H3" si="0">$L$2*B2*$N$2</f>
         <v>5.0258373540000003E-4</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="2">
         <f t="shared" si="0"/>
         <v>2.5083908956000001E-3</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="2">
         <f t="shared" si="0"/>
         <v>2.6725229713500001E-3</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="2">
         <f t="shared" si="0"/>
         <v>2.2842657163E-3</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="2">
         <f t="shared" si="0"/>
         <v>2.8151480854499999E-3</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="2">
         <f t="shared" si="0"/>
         <v>2.84457866455E-3</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="2">
         <f t="shared" si="0"/>
         <v>3.9606767796499997E-3</v>
       </c>
@@ -955,11 +956,11 @@
         <v>25</v>
       </c>
       <c r="B13" s="2">
-        <f t="shared" ref="B13:H13" si="2">(B10+B11*(B9/(1024*1024)/$L$13))*(B6/1000)*B12*$N$2</f>
+        <f>(B10+B11*(B9/(1024*1024)/$L$13))*(B6/1000)*B12*$N$2</f>
         <v>3.3653234201356749E-7</v>
       </c>
       <c r="C13" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="B13:H13" si="2">(C10+C11*(C9/(1024*1024)/$L$13))*(C6/1000)*C12*$N$2</f>
         <v>1.4607142283659242E-6</v>
       </c>
       <c r="D13" s="2">
@@ -1032,31 +1033,31 @@
         <v>27</v>
       </c>
       <c r="B15" s="4">
-        <f t="shared" ref="B15" si="4">SUM(B3,B13,B14)</f>
+        <f>SUM(B3,B13,B14)</f>
         <v>5.5433182455644821E-4</v>
       </c>
       <c r="C15" s="4">
-        <f t="shared" ref="C15" si="5">SUM(C3,C13,C14)</f>
+        <f t="shared" ref="C15" si="4">SUM(C3,C13,C14)</f>
         <v>2.7664888704028536E-3</v>
       </c>
       <c r="D15" s="4">
-        <f t="shared" ref="D15" si="6">SUM(D3,D13,D14)</f>
+        <f t="shared" ref="D15" si="5">SUM(D3,D13,D14)</f>
         <v>2.949856786441309E-3</v>
       </c>
       <c r="E15" s="4">
-        <f t="shared" ref="E15" si="7">SUM(E3,E13,E14)</f>
+        <f t="shared" ref="E15" si="6">SUM(E3,E13,E14)</f>
         <v>2.521466476350129E-3</v>
       </c>
       <c r="F15" s="4">
-        <f t="shared" ref="F15" si="8">SUM(F3,F13,F14)</f>
+        <f t="shared" ref="F15" si="7">SUM(F3,F13,F14)</f>
         <v>3.1132312456202465E-3</v>
       </c>
       <c r="G15" s="4">
-        <f t="shared" ref="G15" si="9">SUM(G3,G13,G14)</f>
+        <f t="shared" ref="G15" si="8">SUM(G3,G13,G14)</f>
         <v>3.2129328311475682E-3</v>
       </c>
       <c r="H15" s="4">
-        <f t="shared" ref="H15" si="10">SUM(H3,H13,H14)</f>
+        <f t="shared" ref="H15" si="9">SUM(H3,H13,H14)</f>
         <v>4.4613110969763687E-3</v>
       </c>
       <c r="I15" s="4">
@@ -1072,36 +1073,36 @@
         <v>28</v>
       </c>
       <c r="B16">
-        <f t="shared" ref="B16:H16" si="11">$L$25*B15</f>
-        <v>0.12029000592874926</v>
+        <f t="shared" ref="B16:H16" si="10">$L$25*B15</f>
+        <v>0.14966959263024102</v>
       </c>
       <c r="C16" s="5">
-        <f t="shared" si="11"/>
-        <v>0.60032808487741929</v>
+        <f t="shared" si="10"/>
+        <v>0.74695199500877052</v>
       </c>
       <c r="D16" s="5">
-        <f t="shared" si="11"/>
-        <v>0.64011892265776404</v>
+        <f t="shared" si="10"/>
+        <v>0.79646133233915339</v>
       </c>
       <c r="E16" s="5">
-        <f t="shared" si="11"/>
-        <v>0.54715822536797798</v>
+        <f t="shared" si="10"/>
+        <v>0.68079594861453485</v>
       </c>
       <c r="F16" s="5">
-        <f t="shared" si="11"/>
-        <v>0.67557118029959351</v>
+        <f t="shared" si="10"/>
+        <v>0.84057243631746659</v>
       </c>
       <c r="G16" s="5">
-        <f t="shared" si="11"/>
-        <v>0.69720642435902236</v>
+        <f t="shared" si="10"/>
+        <v>0.86749186440984338</v>
       </c>
       <c r="H16" s="9">
-        <f t="shared" si="11"/>
-        <v>0.96810450804387205</v>
+        <f t="shared" si="10"/>
+        <v>1.2045539961836196</v>
       </c>
       <c r="I16" s="9">
         <f>SUM(B16:H16)</f>
-        <v>4.2487773515343985</v>
+        <v>5.2864971655036292</v>
       </c>
       <c r="L16" s="10">
         <v>0.1</v>
@@ -1293,19 +1294,19 @@
         <v>1.7600000000000001E-2</v>
       </c>
       <c r="F23">
-        <f t="shared" ref="F23:H23" si="12">(F19+F21)*$L$20</f>
+        <f t="shared" ref="F23:H23" si="11">(F19+F21)*$L$20</f>
         <v>1.7600000000000001E-2</v>
       </c>
       <c r="G23">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>1.7600000000000001E-2</v>
       </c>
       <c r="H23">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>1.7600000000000001E-2</v>
       </c>
       <c r="I23">
-        <f>SUM(B23:H23)</f>
+        <f t="shared" ref="I23:I28" si="12">SUM(B23:H23)</f>
         <v>0.10560000000000001</v>
       </c>
     </row>
@@ -1316,32 +1317,32 @@
       <c r="B24">
         <v>0</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="6">
         <f>C2*$L$36*(1-C20)</f>
         <v>808.39679999999998</v>
       </c>
-      <c r="D24">
-        <f t="shared" ref="D24:H24" si="13">D2*$L$36*(1-D20)</f>
+      <c r="D24" s="6">
+        <f t="shared" ref="D24:F24" si="13">D2*$L$36*(1-D20)</f>
         <v>897.18000000000006</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="6">
         <f t="shared" si="13"/>
         <v>766.84</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="6">
         <f t="shared" si="13"/>
         <v>945.06000000000006</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="6">
         <f>G2*$L$36*(1-G20)</f>
         <v>954.94</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="6">
         <f>H2*$L$36*(1-H20)</f>
         <v>1316.3238000000001</v>
       </c>
-      <c r="I24">
-        <f>SUM(B24:H24)</f>
+      <c r="I24" s="6">
+        <f t="shared" si="12"/>
         <v>5688.7406000000001</v>
       </c>
       <c r="L24" t="s">
@@ -1358,32 +1359,32 @@
       <c r="C25">
         <v>0</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="6">
         <f>($L$32+$L$34)*(D2*$L$28)</f>
         <v>396.64800000000002</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="6">
         <f>($L$32+$L$34)*(E2*$L$28)</f>
         <v>339.024</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="6">
         <f>($L$32+$L$34)*(F2*$L$28)</f>
         <v>417.81600000000003</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="6">
         <f>($L$32+$L$34)*(G2*$L$28)</f>
         <v>422.18400000000003</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="6">
         <f>($L$32+$L$34)*(H2*$L$28)</f>
         <v>587.83199999999999</v>
       </c>
-      <c r="I25">
-        <f>SUM(B25:H25)</f>
+      <c r="I25" s="6">
+        <f t="shared" si="12"/>
         <v>2163.5039999999999</v>
       </c>
       <c r="L25">
-        <v>217</v>
+        <v>270</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -1398,29 +1399,29 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="D26">
-        <f t="shared" si="14"/>
-        <v>2757.6480000000001</v>
-      </c>
-      <c r="E26">
-        <f t="shared" si="14"/>
-        <v>2225.8540000000003</v>
-      </c>
-      <c r="F26">
-        <f t="shared" si="14"/>
-        <v>2904.8159999999998</v>
-      </c>
-      <c r="G26">
-        <f t="shared" si="14"/>
-        <v>2935.1840000000002</v>
-      </c>
-      <c r="H26">
-        <f t="shared" si="14"/>
-        <v>4086.8319999999999</v>
-      </c>
-      <c r="I26">
-        <f>SUM(B26:H26)</f>
-        <v>14910.334000000001</v>
+      <c r="D26" s="6">
+        <f>(1-D22)*D2+D25 - D24</f>
+        <v>1860.4680000000001</v>
+      </c>
+      <c r="E26" s="6">
+        <f t="shared" ref="E26:H26" si="15">(1-E22)*E2+E25 - E24</f>
+        <v>1459.0140000000001</v>
+      </c>
+      <c r="F26" s="6">
+        <f t="shared" si="15"/>
+        <v>1959.7559999999999</v>
+      </c>
+      <c r="G26" s="6">
+        <f t="shared" si="15"/>
+        <v>1980.2440000000001</v>
+      </c>
+      <c r="H26" s="6">
+        <f t="shared" si="15"/>
+        <v>2770.5081999999998</v>
+      </c>
+      <c r="I26" s="6">
+        <f t="shared" si="12"/>
+        <v>10029.9902</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -1432,32 +1433,32 @@
         <v>2.2000000000000001E-3</v>
       </c>
       <c r="C27" s="5">
-        <f t="shared" ref="C27:H27" si="15">C23+(C24+C26)*$L$2*$N$2</f>
+        <f>C23+(C24+C26)*$L$2*$N$2</f>
         <v>1.6315060998714881E-2</v>
       </c>
       <c r="D27" s="5">
-        <f t="shared" si="15"/>
-        <v>2.1737065559649802E-2</v>
+        <f>D23+(D24+D26)*$L$2*$N$2</f>
+        <v>2.07215068305368E-2</v>
       </c>
       <c r="E27" s="5">
-        <f t="shared" si="15"/>
-        <v>2.0987566057272901E-2</v>
-      </c>
-      <c r="F27">
-        <f t="shared" si="15"/>
-        <v>2.19578492362766E-2</v>
-      </c>
-      <c r="G27" s="4">
-        <f t="shared" si="15"/>
-        <v>2.2003407772723402E-2</v>
-      </c>
-      <c r="H27">
-        <f t="shared" si="15"/>
-        <v>2.3716077083135532E-2</v>
-      </c>
-      <c r="I27">
-        <f>SUM(B27:H27)</f>
-        <v>0.12891702670777314</v>
+        <f t="shared" ref="C27:H27" si="16">E23+(E24+E26)*$L$2*$N$2</f>
+        <v>2.0119545085078901E-2</v>
+      </c>
+      <c r="F27" s="5">
+        <f t="shared" si="16"/>
+        <v>2.0888092963805602E-2</v>
+      </c>
+      <c r="G27" s="5">
+        <f t="shared" si="16"/>
+        <v>2.09224678801944E-2</v>
+      </c>
+      <c r="H27" s="5">
+        <f t="shared" si="16"/>
+        <v>2.2226070478631201E-2</v>
+      </c>
+      <c r="I27" s="5">
+        <f t="shared" si="12"/>
+        <v>0.1233927442369618</v>
       </c>
       <c r="L27" t="s">
         <v>38</v>
@@ -1469,35 +1470,35 @@
       </c>
       <c r="B28">
         <f>B27*$L$25</f>
-        <v>0.47740000000000005</v>
-      </c>
-      <c r="C28">
-        <f t="shared" ref="C28:H28" si="16">C27*$L$25</f>
-        <v>3.5403682367211293</v>
-      </c>
-      <c r="D28">
-        <f t="shared" si="16"/>
-        <v>4.7169432264440072</v>
-      </c>
-      <c r="E28">
-        <f t="shared" si="16"/>
-        <v>4.5543018344282196</v>
-      </c>
-      <c r="F28">
-        <f t="shared" si="16"/>
-        <v>4.7648532842720224</v>
-      </c>
-      <c r="G28">
-        <f t="shared" si="16"/>
-        <v>4.7747394866809785</v>
-      </c>
-      <c r="H28">
-        <f t="shared" si="16"/>
-        <v>5.1463887270404101</v>
-      </c>
-      <c r="I28">
-        <f>SUM(B28:H28)</f>
-        <v>27.974994795586767</v>
+        <v>0.59400000000000008</v>
+      </c>
+      <c r="C28" s="9">
+        <f t="shared" ref="C28:H28" si="17">C27*$L$25</f>
+        <v>4.4050664696530175</v>
+      </c>
+      <c r="D28" s="9">
+        <f t="shared" si="17"/>
+        <v>5.5948068442449364</v>
+      </c>
+      <c r="E28" s="9">
+        <f t="shared" si="17"/>
+        <v>5.4322771729713031</v>
+      </c>
+      <c r="F28" s="9">
+        <f t="shared" si="17"/>
+        <v>5.6397851002275123</v>
+      </c>
+      <c r="G28" s="9">
+        <f t="shared" si="17"/>
+        <v>5.6490663276524877</v>
+      </c>
+      <c r="H28" s="9">
+        <f t="shared" si="17"/>
+        <v>6.0010390292304248</v>
+      </c>
+      <c r="I28" s="11">
+        <f t="shared" si="12"/>
+        <v>33.316040943979687</v>
       </c>
       <c r="L28" s="10">
         <v>0.42</v>

</xml_diff>